<commit_message>
Get to Windows, Added windows support
</commit_message>
<xml_diff>
--- a/documentation/test-cases/test-cases.xlsx
+++ b/documentation/test-cases/test-cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t xml:space="preserve">Online Storage Test Cases</t>
   </si>
@@ -34,7 +34,10 @@
     <t xml:space="preserve">Assigned To</t>
   </si>
   <si>
-    <t xml:space="preserve">User Registration</t>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Registration – Valid Inputs</t>
   </si>
   <si>
     <t xml:space="preserve">Tc#1</t>
@@ -43,25 +46,82 @@
     <t xml:space="preserve">Umer Farooq</t>
   </si>
   <si>
-    <t xml:space="preserve">Login</t>
+    <t xml:space="preserve">Try to register to system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Registration – Invalid Inputs(Existing Email)</t>
   </si>
   <si>
     <t xml:space="preserve">Tc#2</t>
   </si>
   <si>
+    <t xml:space="preserve">Try to register to system with existing email and/or invalid inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Login – Valid Inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tc#3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Faisal Shahzad</t>
   </si>
   <si>
-    <t xml:space="preserve">User Panel Toolbar Functionality Check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tc#3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Panel File System Entry Functionality Check</t>
+    <t xml:space="preserve">Try to login to system with a valid email and password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Login – Invalid Inputs(either invalid email or password or both)</t>
   </si>
   <si>
     <t xml:space="preserve">Tc#4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to login to system with an invalid email and/or password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Panel – Toolbar Navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tc#5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open a directory, then try to go back, and then go forward using ← or → button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Panel – Copy/Cut and Paste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tc#6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select some files/directories and try to copy and cut them and paste in another directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Panel – Delete and Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tc#7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select some files/directories and try to delete them using Delete button at top and then logout.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Panel – Open Directory and Delete Directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tc#8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open a directory, get back and delete same directory  using delete button on directory bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Panel – File Working Checking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tc#9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open a file by clicking on it, close it, download it and then delete it using buttons with it.</t>
   </si>
 </sst>
 </file>
@@ -76,6 +136,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -104,6 +165,7 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,17 +244,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="85.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="80.03"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -210,49 +273,134 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B12" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>9</v>
+      <c r="C12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>